<commit_message>
adding comments and edits to dedicated project folder
Mike's comments, Lauren's edits, moving things around to organise things better
</commit_message>
<xml_diff>
--- a/ms/final model output and tables/Supplementary_models_S1-S6.xlsx
+++ b/ms/final model output and tables/Supplementary_models_S1-S6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_meta/ms/final model output and tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970296BF-2FD6-AC46-9BB6-579A10CA2C8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751B837F-B607-6846-A5AF-4183B6AF6B7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="460" windowWidth="38200" windowHeight="19700" xr2:uid="{5BDBDF95-A114-D34B-9842-3CB243171EE0}"/>
   </bookViews>
@@ -1665,9 +1665,6 @@
     <t>Here we include the random effects: study_ID (between study variance), phylo (phylogenetic variance) and obs (observation-level random effect - within study variance)</t>
   </si>
   <si>
-    <t>obs - observation-level random effect where each effect size from the same study is given a numeric value.</t>
-  </si>
-  <si>
     <t xml:space="preserve">I2 measures of heterogeneity are explained in the metadata on sheet 1. </t>
   </si>
   <si>
@@ -1777,6 +1774,9 @@
   </si>
   <si>
     <t>I2 study - proportion of heterogeneity explained by study effects</t>
+  </si>
+  <si>
+    <t>obs - observation-level random effect where each effect size from the same study is given a unique numeric value.</t>
   </si>
 </sst>
 </file>
@@ -2262,14 +2262,14 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -2279,32 +2279,32 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
@@ -2314,57 +2314,57 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>544</v>
+        <v>581</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -2391,13 +2391,13 @@
   <sheetData>
     <row r="1" spans="1:34" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
@@ -2407,7 +2407,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -3050,7 +3050,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F16" s="9" t="s">
         <v>19</v>
@@ -3067,7 +3067,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="M16" s="9" t="s">
         <v>19</v>
@@ -3084,7 +3084,7 @@
         <v>23</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="T16" s="9" t="s">
         <v>19</v>
@@ -3101,7 +3101,7 @@
         <v>23</v>
       </c>
       <c r="Z16" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AA16" s="9" t="s">
         <v>19</v>
@@ -3118,7 +3118,7 @@
         <v>23</v>
       </c>
       <c r="AG16" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AH16" s="9" t="s">
         <v>19</v>
@@ -3821,7 +3821,7 @@
         <v>23</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>19</v>
@@ -3838,7 +3838,7 @@
         <v>23</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="M28" s="9" t="s">
         <v>19</v>
@@ -3855,7 +3855,7 @@
         <v>23</v>
       </c>
       <c r="S28" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="T28" s="9" t="s">
         <v>19</v>
@@ -3872,7 +3872,7 @@
         <v>23</v>
       </c>
       <c r="Z28" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AA28" s="9" t="s">
         <v>19</v>
@@ -3889,7 +3889,7 @@
         <v>23</v>
       </c>
       <c r="AG28" s="8" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AH28" s="9" t="s">
         <v>19</v>
@@ -4201,23 +4201,23 @@
   <sheetData>
     <row r="1" spans="1:45" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:45" s="11" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -4792,7 +4792,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>23</v>
@@ -4817,7 +4817,7 @@
         <v>34</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>23</v>
@@ -4842,7 +4842,7 @@
         <v>34</v>
       </c>
       <c r="V15" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="W15" s="8" t="s">
         <v>23</v>
@@ -4867,7 +4867,7 @@
         <v>34</v>
       </c>
       <c r="AE15" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AF15" s="8" t="s">
         <v>23</v>
@@ -4892,7 +4892,7 @@
         <v>34</v>
       </c>
       <c r="AN15" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AO15" s="8" t="s">
         <v>23</v>
@@ -6108,7 +6108,7 @@
         <v>34</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>23</v>
@@ -6132,7 +6132,7 @@
         <v>34</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="N30" s="17" t="s">
         <v>23</v>
@@ -6156,7 +6156,7 @@
         <v>34</v>
       </c>
       <c r="V30" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="W30" s="17" t="s">
         <v>23</v>
@@ -6180,7 +6180,7 @@
         <v>34</v>
       </c>
       <c r="AE30" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AF30" s="17" t="s">
         <v>23</v>
@@ -6204,7 +6204,7 @@
         <v>34</v>
       </c>
       <c r="AN30" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AO30" s="17" t="s">
         <v>23</v>
@@ -6937,13 +6937,13 @@
   <sheetData>
     <row r="1" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:49" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="43"/>
@@ -6996,7 +6996,7 @@
     </row>
     <row r="3" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B3"/>
       <c r="K3" s="19"/>
@@ -7006,7 +7006,7 @@
     </row>
     <row r="4" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B4"/>
       <c r="K4" s="22"/>
@@ -12035,13 +12035,13 @@
   <sheetData>
     <row r="1" spans="1:49" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:49" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B2"/>
       <c r="C2" s="43"/>
@@ -12094,7 +12094,7 @@
     </row>
     <row r="3" spans="1:49" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B3"/>
       <c r="K3" s="19"/>
@@ -16331,18 +16331,18 @@
   <sheetData>
     <row r="1" spans="1:40" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
@@ -19060,13 +19060,13 @@
   <sheetData>
     <row r="1" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>